<commit_message>
Update States to Hex Truth Tables.xlsx
</commit_message>
<xml_diff>
--- a/States to Hex Truth Tables.xlsx
+++ b/States to Hex Truth Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilr\Desktop\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B590AA73-AAED-4FB6-9F60-7F678344D231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C7288D-9C29-4EFE-8F25-313ACF001D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2745" windowWidth="29040" windowHeight="15840" xr2:uid="{13F4B11F-993E-4BCF-B4D2-908CE3D19F6E}"/>
+    <workbookView xWindow="-28920" yWindow="2790" windowWidth="29040" windowHeight="15840" xr2:uid="{13F4B11F-993E-4BCF-B4D2-908CE3D19F6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>State to Hex Truth Table</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>C11</t>
+  </si>
+  <si>
+    <t>HEX 3</t>
+  </si>
+  <si>
+    <t>HEX 4</t>
+  </si>
+  <si>
+    <t>HEX 5</t>
   </si>
 </sst>
 </file>
@@ -257,7 +266,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -266,13 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,103 +601,103 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.140625" style="11"/>
+    <col min="1" max="7" width="9.140625" style="8"/>
     <col min="8" max="11" width="9.140625" style="5"/>
-    <col min="12" max="15" width="9.140625" style="11"/>
+    <col min="12" max="15" width="9.140625" style="8"/>
     <col min="16" max="19" width="9.140625" style="5"/>
     <col min="21" max="21" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="9" t="s">
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1026,90 +1035,90 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="12" t="s">
+      <c r="M13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="N13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="O13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R13" s="13" t="s">
+      <c r="R13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="S13" s="10" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>